<commit_message>
Latest measures. Re-enable Airflow EnergyPlus measure.
</commit_message>
<xml_diff>
--- a/projects/resstock_pnw.xlsx
+++ b/projects/resstock_pnw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="473">
   <si>
     <t>type</t>
   </si>
@@ -1435,6 +1435,24 @@
   </si>
   <si>
     <t>1.20.1</t>
+  </si>
+  <si>
+    <t>Build Existing Models EnergyPlus</t>
+  </si>
+  <si>
+    <t>BuildExistingModelEnergyPlus</t>
+  </si>
+  <si>
+    <t>EnergyPlusMeasure</t>
+  </si>
+  <si>
+    <t>Always Run</t>
+  </si>
+  <si>
+    <t>always_run</t>
+  </si>
+  <si>
+    <t>[1]</t>
   </si>
 </sst>
 </file>
@@ -3563,7 +3581,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3664,6 +3682,10 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1544">
     <cellStyle name="20% - Accent1" xfId="1521" builtinId="30" customBuiltin="1"/>
@@ -5510,7 +5532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6015,9 +6037,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6277,153 +6301,165 @@
       <c r="W5" s="45"/>
       <c r="X5" s="45"/>
     </row>
-    <row r="6" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>467</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>468</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>468</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>469</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="52"/>
+      <c r="Z6" s="52"/>
+    </row>
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="54" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54" t="s">
+        <v>470</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>471</v>
+      </c>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54" t="s">
+        <v>267</v>
+      </c>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54">
+        <v>1</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54">
+        <v>1</v>
+      </c>
+      <c r="L7" s="54">
+        <v>1</v>
+      </c>
+      <c r="M7" s="54">
+        <v>1</v>
+      </c>
+      <c r="N7" s="54">
+        <v>1</v>
+      </c>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="S7" s="54"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="54"/>
+      <c r="V7" s="54"/>
+      <c r="W7" s="54"/>
+      <c r="X7" s="54"/>
+      <c r="Y7" s="55"/>
+      <c r="Z7" s="55"/>
+    </row>
+    <row r="8" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>272</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C8" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D8" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E8" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-    </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="45" t="s">
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+    </row>
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D7" s="45" t="str">
-        <f>"Run " &amp; B6</f>
+      <c r="D9" s="45" t="str">
+        <f>"Run " &amp; B8</f>
         <v>Run R60 Attic Insulation Upgrade</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E9" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G9" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="I7" s="45">
+      <c r="I9" s="45">
         <v>1</v>
       </c>
-      <c r="K7" s="45">
-        <v>0</v>
-      </c>
-      <c r="L7" s="45">
+      <c r="K9" s="45">
+        <v>0</v>
+      </c>
+      <c r="L9" s="45">
         <v>1</v>
       </c>
-      <c r="M7" s="45">
+      <c r="M9" s="45">
         <v>1</v>
       </c>
-      <c r="N7" s="45">
+      <c r="N9" s="45">
         <v>1</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P9" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="R7" s="45" t="s">
+      <c r="R9" s="45" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -6432,10 +6468,10 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>273</v>
+        <v>449</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>274</v>
+        <v>447</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
@@ -6443,7 +6479,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6463,153 +6499,153 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+    </row>
+    <row r="13" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>282</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C13" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D13" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E13" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
-      <c r="W11" s="39"/>
-      <c r="X11" s="39"/>
-    </row>
-    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+    </row>
+    <row r="14" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="45" t="str">
-        <f>"Run " &amp; B11</f>
+      <c r="D14" s="45" t="str">
+        <f>"Run " &amp; B13</f>
         <v>Run Triple-Pane Windows Upgrade</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E14" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G14" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="I12" s="45">
+      <c r="I14" s="45">
         <v>1</v>
       </c>
-      <c r="K12" s="45">
-        <v>0</v>
-      </c>
-      <c r="L12" s="45">
+      <c r="K14" s="45">
+        <v>0</v>
+      </c>
+      <c r="L14" s="45">
         <v>1</v>
       </c>
-      <c r="M12" s="45">
+      <c r="M14" s="45">
         <v>1</v>
       </c>
-      <c r="N12" s="45">
+      <c r="N14" s="45">
         <v>1</v>
       </c>
-      <c r="P12" s="45" t="s">
+      <c r="P14" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="R12" s="45" t="s">
+      <c r="R14" s="45" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-    </row>
-    <row r="14" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
     </row>
     <row r="15" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
@@ -6618,10 +6654,10 @@
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>273</v>
+        <v>449</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>274</v>
+        <v>447</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
@@ -6629,7 +6665,7 @@
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -6649,153 +6685,153 @@
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="39" t="s">
+    <row r="16" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+    </row>
+    <row r="17" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+    </row>
+    <row r="18" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C18" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D18" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E18" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="39"/>
-      <c r="V16" s="39"/>
-      <c r="W16" s="39"/>
-      <c r="X16" s="39"/>
-    </row>
-    <row r="17" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="39"/>
+      <c r="X18" s="39"/>
+    </row>
+    <row r="19" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="45" t="str">
-        <f>"Run " &amp; B16</f>
+      <c r="D19" s="45" t="str">
+        <f>"Run " &amp; B18</f>
         <v>Run LED Lighting Upgrade</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E19" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G19" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="I17" s="45">
+      <c r="I19" s="45">
         <v>1</v>
       </c>
-      <c r="K17" s="45">
-        <v>0</v>
-      </c>
-      <c r="L17" s="45">
+      <c r="K19" s="45">
+        <v>0</v>
+      </c>
+      <c r="L19" s="45">
         <v>1</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M19" s="45">
         <v>1</v>
       </c>
-      <c r="N17" s="45">
+      <c r="N19" s="45">
         <v>1</v>
       </c>
-      <c r="P17" s="45" t="s">
+      <c r="P19" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="R17" s="45" t="s">
+      <c r="R19" s="45" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-    </row>
-    <row r="19" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
@@ -6804,10 +6840,10 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>273</v>
+        <v>449</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>274</v>
+        <v>447</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
@@ -6815,7 +6851,7 @@
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -6835,153 +6871,153 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="39" t="s">
+    <row r="21" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+    </row>
+    <row r="22" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+    </row>
+    <row r="23" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" s="39" t="s">
         <v>281</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C23" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D23" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E23" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-    </row>
-    <row r="22" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="39"/>
+    </row>
+    <row r="24" spans="1:26" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="D22" s="45" t="str">
-        <f>"Run " &amp; B21</f>
+      <c r="D24" s="45" t="str">
+        <f>"Run " &amp; B23</f>
         <v>Run Attic+Windows+Lighting Package</v>
       </c>
-      <c r="E22" s="45" t="s">
+      <c r="E24" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G24" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="I22" s="45">
+      <c r="I24" s="45">
         <v>1</v>
       </c>
-      <c r="K22" s="45">
-        <v>0</v>
-      </c>
-      <c r="L22" s="45">
+      <c r="K24" s="45">
+        <v>0</v>
+      </c>
+      <c r="L24" s="45">
         <v>1</v>
       </c>
-      <c r="M22" s="45">
+      <c r="M24" s="45">
         <v>1</v>
       </c>
-      <c r="N22" s="45">
+      <c r="N24" s="45">
         <v>1</v>
       </c>
-      <c r="P22" s="45" t="s">
+      <c r="P24" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="R22" s="45" t="s">
+      <c r="R24" s="45" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-    </row>
-    <row r="24" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
     </row>
     <row r="25" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
@@ -6990,10 +7026,10 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>273</v>
+        <v>449</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>274</v>
+        <v>447</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
@@ -7001,7 +7037,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>275</v>
+        <v>445</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7021,90 +7057,94 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>374</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>375</v>
-      </c>
-      <c r="D26" s="40" t="s">
-        <v>375</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="40"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="40"/>
-      <c r="X26" s="40"/>
-    </row>
-    <row r="27" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>353</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>354</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>354</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="40"/>
-      <c r="U27" s="40"/>
-      <c r="V27" s="40"/>
-      <c r="W27" s="40"/>
-      <c r="X27" s="40"/>
+    <row r="26" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
+    </row>
+    <row r="27" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
     </row>
     <row r="28" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="b">
         <v>1</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>238</v>
+        <v>374</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>237</v>
+        <v>375</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>237</v>
+        <v>375</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>236</v>
@@ -7129,11 +7169,83 @@
       <c r="W28" s="40"/>
       <c r="X28" s="40"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
+    <row r="29" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+    </row>
+    <row r="30" spans="1:26" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="40"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B31" s="50"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B32" s="50"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>

</xml_diff>

<commit_message>
Added Geometry Heated Basement to PNW output csv.
</commit_message>
<xml_diff>
--- a/projects/resstock_pnw.xlsx
+++ b/projects/resstock_pnw.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="472">
   <si>
     <t>type</t>
   </si>
@@ -1444,6 +1444,12 @@
   </si>
   <si>
     <t>Insulation Wall|Wood Stud, Uninsulated &amp;&amp; (Windows|Clear, Single, Metal || Windows|Clear, Single, Non-metal)</t>
+  </si>
+  <si>
+    <t>Geometry Heated Basement</t>
+  </si>
+  <si>
+    <t>building_characteristics_report.Geometry Heated Basement</t>
   </si>
 </sst>
 </file>
@@ -7410,7 +7416,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -7719,12 +7725,12 @@
     </row>
     <row r="11" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>285</v>
+        <v>470</v>
       </c>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="D11" s="48" t="s">
-        <v>368</v>
+        <v>471</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="48" t="s">
@@ -7746,12 +7752,12 @@
     </row>
     <row r="12" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="48" t="s">
@@ -7773,12 +7779,12 @@
     </row>
     <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="48" t="s">
@@ -7800,12 +7806,12 @@
     </row>
     <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>438</v>
+        <v>287</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="48" t="s">
-        <v>439</v>
+        <v>370</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="48" t="s">
@@ -7827,12 +7833,12 @@
     </row>
     <row r="15" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>288</v>
+        <v>438</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
       <c r="D15" s="48" t="s">
-        <v>371</v>
+        <v>439</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
@@ -7854,12 +7860,12 @@
     </row>
     <row r="16" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
       <c r="D16" s="48" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
@@ -7881,12 +7887,12 @@
     </row>
     <row r="17" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
       <c r="D17" s="48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="48" t="s">
@@ -7908,11 +7914,14 @@
     </row>
     <row r="18" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>291</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="48" t="s">
-        <v>374</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="E18" s="48"/>
       <c r="F18" s="48" t="s">
         <v>244</v>
       </c>
@@ -7925,13 +7934,17 @@
       <c r="I18" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
     </row>
     <row r="19" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F19" s="48" t="s">
         <v>244</v>
@@ -7948,14 +7961,11 @@
     </row>
     <row r="20" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
-        <v>293</v>
-      </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
+        <v>292</v>
+      </c>
       <c r="D20" s="48" t="s">
-        <v>376</v>
-      </c>
-      <c r="E20" s="48"/>
+        <v>375</v>
+      </c>
       <c r="F20" s="48" t="s">
         <v>244</v>
       </c>
@@ -7968,19 +7978,15 @@
       <c r="I20" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
       <c r="D21" s="48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E21" s="48"/>
       <c r="F21" s="48" t="s">
@@ -8002,12 +8008,12 @@
     </row>
     <row r="22" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E22" s="48"/>
       <c r="F22" s="48" t="s">
@@ -8029,12 +8035,12 @@
     </row>
     <row r="23" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E23" s="48"/>
       <c r="F23" s="48" t="s">
@@ -8056,12 +8062,12 @@
     </row>
     <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="48" t="s">
@@ -8083,11 +8089,14 @@
     </row>
     <row r="25" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
-        <v>297</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="48" t="s">
-        <v>381</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="E25" s="48"/>
       <c r="F25" s="48" t="s">
         <v>244</v>
       </c>
@@ -8100,13 +8109,17 @@
       <c r="I25" s="48" t="b">
         <v>0</v>
       </c>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F26" s="48" t="s">
         <v>244</v>
@@ -8123,10 +8136,10 @@
     </row>
     <row r="27" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F27" s="48" t="s">
         <v>244</v>
@@ -8143,10 +8156,10 @@
     </row>
     <row r="28" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F28" s="48" t="s">
         <v>244</v>
@@ -8163,10 +8176,10 @@
     </row>
     <row r="29" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F29" s="48" t="s">
         <v>244</v>
@@ -8183,10 +8196,10 @@
     </row>
     <row r="30" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F30" s="48" t="s">
         <v>244</v>
@@ -8203,10 +8216,10 @@
     </row>
     <row r="31" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F31" s="48" t="s">
         <v>244</v>
@@ -8223,10 +8236,10 @@
     </row>
     <row r="32" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D32" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F32" s="48" t="s">
         <v>244</v>
@@ -8243,10 +8256,10 @@
     </row>
     <row r="33" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F33" s="48" t="s">
         <v>244</v>
@@ -8263,10 +8276,10 @@
     </row>
     <row r="34" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F34" s="48" t="s">
         <v>244</v>
@@ -8283,10 +8296,10 @@
     </row>
     <row r="35" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F35" s="48" t="s">
         <v>244</v>
@@ -8303,10 +8316,10 @@
     </row>
     <row r="36" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F36" s="48" t="s">
         <v>244</v>
@@ -8323,10 +8336,10 @@
     </row>
     <row r="37" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F37" s="48" t="s">
         <v>244</v>
@@ -8343,10 +8356,10 @@
     </row>
     <row r="38" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>244</v>
@@ -8363,10 +8376,10 @@
     </row>
     <row r="39" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F39" s="48" t="s">
         <v>244</v>
@@ -8383,10 +8396,10 @@
     </row>
     <row r="40" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F40" s="48" t="s">
         <v>244</v>
@@ -8403,10 +8416,10 @@
     </row>
     <row r="41" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F41" s="48" t="s">
         <v>244</v>
@@ -8423,10 +8436,10 @@
     </row>
     <row r="42" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="D42" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F42" s="48" t="s">
         <v>244</v>
@@ -8443,10 +8456,10 @@
     </row>
     <row r="43" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
-        <v>314</v>
+        <v>272</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F43" s="48" t="s">
         <v>244</v>
@@ -8463,10 +8476,10 @@
     </row>
     <row r="44" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F44" s="48" t="s">
         <v>244</v>
@@ -8483,10 +8496,10 @@
     </row>
     <row r="45" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="48" t="s">
-        <v>431</v>
+        <v>315</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>432</v>
+        <v>400</v>
       </c>
       <c r="F45" s="48" t="s">
         <v>244</v>
@@ -8503,10 +8516,10 @@
     </row>
     <row r="46" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48" t="s">
-        <v>316</v>
+        <v>431</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>401</v>
+        <v>432</v>
       </c>
       <c r="F46" s="48" t="s">
         <v>244</v>
@@ -8523,10 +8536,10 @@
     </row>
     <row r="47" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F47" s="48" t="s">
         <v>244</v>
@@ -8543,10 +8556,10 @@
     </row>
     <row r="48" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F48" s="48" t="s">
         <v>244</v>
@@ -8563,10 +8576,10 @@
     </row>
     <row r="49" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F49" s="48" t="s">
         <v>244</v>
@@ -8583,10 +8596,10 @@
     </row>
     <row r="50" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F50" s="48" t="s">
         <v>244</v>
@@ -8603,10 +8616,10 @@
     </row>
     <row r="51" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F51" s="48" t="s">
         <v>244</v>
@@ -8623,10 +8636,10 @@
     </row>
     <row r="52" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F52" s="48" t="s">
         <v>244</v>
@@ -8643,10 +8656,10 @@
     </row>
     <row r="53" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F53" s="48" t="s">
         <v>244</v>
@@ -8663,10 +8676,10 @@
     </row>
     <row r="54" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F54" s="48" t="s">
         <v>244</v>
@@ -8683,10 +8696,10 @@
     </row>
     <row r="55" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D55" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F55" s="48" t="s">
         <v>244</v>
@@ -8703,10 +8716,10 @@
     </row>
     <row r="56" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D56" s="48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F56" s="48" t="s">
         <v>244</v>
@@ -8723,10 +8736,10 @@
     </row>
     <row r="57" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
-        <v>273</v>
+        <v>326</v>
       </c>
       <c r="D57" s="48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F57" s="48" t="s">
         <v>244</v>
@@ -8743,10 +8756,10 @@
     </row>
     <row r="58" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
-        <v>327</v>
+        <v>273</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F58" s="48" t="s">
         <v>244</v>
@@ -8763,10 +8776,10 @@
     </row>
     <row r="59" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F59" s="48" t="s">
         <v>244</v>
@@ -8783,10 +8796,10 @@
     </row>
     <row r="60" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F60" s="48" t="s">
         <v>244</v>
@@ -8803,10 +8816,10 @@
     </row>
     <row r="61" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F61" s="48" t="s">
         <v>244</v>
@@ -8823,10 +8836,10 @@
     </row>
     <row r="62" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F62" s="48" t="s">
         <v>244</v>
@@ -8843,10 +8856,10 @@
     </row>
     <row r="63" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F63" s="48" t="s">
         <v>244</v>
@@ -8863,10 +8876,10 @@
     </row>
     <row r="64" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F64" s="48" t="s">
         <v>244</v>
@@ -8883,10 +8896,10 @@
     </row>
     <row r="65" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D65" s="48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F65" s="48" t="s">
         <v>244</v>
@@ -8903,10 +8916,10 @@
     </row>
     <row r="66" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D66" s="48" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F66" s="48" t="s">
         <v>244</v>
@@ -8923,10 +8936,10 @@
     </row>
     <row r="67" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D67" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F67" s="48" t="s">
         <v>244</v>
@@ -8943,10 +8956,10 @@
     </row>
     <row r="68" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D68" s="48" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F68" s="48" t="s">
         <v>244</v>
@@ -8963,10 +8976,10 @@
     </row>
     <row r="69" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D69" s="48" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>244</v>
@@ -8983,10 +8996,10 @@
     </row>
     <row r="70" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D70" s="48" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>244</v>
@@ -9001,32 +9014,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
-        <v>245</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="G71" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H71" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I71" s="14" t="b">
+    <row r="71" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="48" t="s">
+        <v>339</v>
+      </c>
+      <c r="D71" s="48" t="s">
+        <v>425</v>
+      </c>
+      <c r="F71" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="G71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" s="48" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>426</v>
@@ -9043,10 +9056,10 @@
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>426</v>
@@ -9063,10 +9076,10 @@
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>426</v>
@@ -9083,10 +9096,10 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>426</v>
@@ -9103,10 +9116,10 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>426</v>
@@ -9123,10 +9136,10 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>426</v>
@@ -9143,10 +9156,10 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>426</v>
@@ -9163,10 +9176,10 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>426</v>
@@ -9183,10 +9196,10 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>426</v>
@@ -9203,10 +9216,10 @@
     </row>
     <row r="81" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F81" s="14" t="s">
         <v>426</v>
@@ -9223,10 +9236,10 @@
     </row>
     <row r="82" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F82" s="14" t="s">
         <v>426</v>
@@ -9242,11 +9255,11 @@
       </c>
     </row>
     <row r="83" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>257</v>
+      <c r="A83" s="49" t="s">
+        <v>256</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F83" s="14" t="s">
         <v>426</v>
@@ -9263,10 +9276,10 @@
     </row>
     <row r="84" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F84" s="14" t="s">
         <v>426</v>
@@ -9283,10 +9296,10 @@
     </row>
     <row r="85" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F85" s="14" t="s">
         <v>426</v>
@@ -9303,10 +9316,10 @@
     </row>
     <row r="86" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F86" s="14" t="s">
         <v>426</v>
@@ -9323,10 +9336,10 @@
     </row>
     <row r="87" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F87" s="14" t="s">
         <v>426</v>
@@ -9343,10 +9356,10 @@
     </row>
     <row r="88" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>426</v>
@@ -9363,10 +9376,10 @@
     </row>
     <row r="89" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>434</v>
+        <v>262</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>435</v>
+        <v>359</v>
       </c>
       <c r="F89" s="14" t="s">
         <v>426</v>
@@ -9380,17 +9393,13 @@
       <c r="I89" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="J89" s="49"/>
-      <c r="K89" s="49"/>
-      <c r="L89" s="49"/>
-      <c r="M89" s="49"/>
     </row>
     <row r="90" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>426</v>
@@ -9410,11 +9419,11 @@
       <c r="M90" s="49"/>
     </row>
     <row r="91" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
-        <v>440</v>
+      <c r="A91" s="14" t="s">
+        <v>436</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F91" s="14" t="s">
         <v>426</v>
@@ -9428,13 +9437,17 @@
       <c r="I91" s="14" t="b">
         <v>0</v>
       </c>
+      <c r="J91" s="49"/>
+      <c r="K91" s="49"/>
+      <c r="L91" s="49"/>
+      <c r="M91" s="49"/>
     </row>
     <row r="92" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="49" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>426</v>
@@ -9449,14 +9462,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-      <c r="B93" s="21"/>
-      <c r="D93" s="15"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
-      <c r="I93" s="15"/>
+    <row r="93" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="49" t="s">
+        <v>441</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="G93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
@@ -9710,12 +9734,10 @@
       <c r="H121" s="15"/>
       <c r="I121" s="15"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122" s="21"/>
-      <c r="C122" s="22"/>
       <c r="D122" s="15"/>
-      <c r="E122" s="22"/>
       <c r="F122" s="15"/>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
@@ -9775,6 +9797,17 @@
       <c r="G127" s="15"/>
       <c r="H127" s="15"/>
       <c r="I127" s="15"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="15"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="22"/>
+      <c r="D128" s="15"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="15"/>
+      <c r="H128" s="15"/>
+      <c r="I128" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added more parameters to data\rbsa\output.py script.
Updated resstock_pnw.xlsx to 10k simulations. Error out on upgrades that don't apply to reduce runtime.

Latest measures.
</commit_message>
<xml_diff>
--- a/projects/resstock_pnw.xlsx
+++ b/projects/resstock_pnw.xlsx
@@ -5617,7 +5617,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="21">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>362</v>
@@ -5791,7 +5791,7 @@
       </c>
       <c r="C45" s="2" t="str">
         <f>"['pnw'," &amp; B24 &amp; "]"</f>
-        <v>['pnw',1000]</v>
+        <v>['pnw',10000]</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
@@ -6081,7 +6081,7 @@
       </c>
       <c r="L5" s="45">
         <f>Setup!B24</f>
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="M5" s="45">
         <v>1</v>

</xml_diff>

<commit_message>
Added PNW 10k results. Added cooling climate zones to the calibration graphs.
</commit_message>
<xml_diff>
--- a/projects/resstock_pnw.xlsx
+++ b/projects/resstock_pnw.xlsx
@@ -5334,7 +5334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5461,7 +5463,7 @@
         <v>66</v>
       </c>
       <c r="B9" s="16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5469,7 +5471,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$5.04/hour</v>
+        <v>$10.08/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>201</v>

</xml_diff>